<commit_message>
bad eval data table solution
</commit_message>
<xml_diff>
--- a/other documents/experiment-data.xlsx
+++ b/other documents/experiment-data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lop1le\Documents\Master-Thesis\template-thesis-template-rss\other documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FDE0C0-F7AF-45C7-9773-FAA004BEE9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCB7A0D-B1FE-450C-8CCF-F2B5C3868476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="3" xr2:uid="{74E725B0-5B7F-4207-B493-632C2DD28F84}"/>
+    <workbookView xWindow="-38520" yWindow="-7935" windowWidth="38640" windowHeight="21240" xr2:uid="{74E725B0-5B7F-4207-B493-632C2DD28F84}"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
     <sheet name="tasks" sheetId="2" r:id="rId2"/>
-    <sheet name="qual" sheetId="3" r:id="rId3"/>
-    <sheet name="quan" sheetId="4" r:id="rId4"/>
+    <sheet name="quan" sheetId="3" r:id="rId3"/>
+    <sheet name="qual" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>job</t>
   </si>
@@ -125,15 +125,9 @@
     <t>Q6</t>
   </si>
   <si>
-    <t>Q7</t>
-  </si>
-  <si>
     <t>finance/bank</t>
   </si>
   <si>
-    <t>few</t>
-  </si>
-  <si>
     <t>Wenn er Geräte steuern sollte und es nicht macht</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>automatisch vorschläge / tipps zur optimierung des Verhaltens. (nutzungsverhalten, stromverbrauch…)</t>
   </si>
   <si>
-    <t>infromatiker</t>
-  </si>
-  <si>
     <t xml:space="preserve">Antworten manchmal kontext bezogen (historienbasiert) obwohl es keinen sinn macht. </t>
   </si>
   <si>
@@ -159,19 +150,59 @@
   </si>
   <si>
     <t>Routinen erstellen für Standy von geräten erkennen wenn wenig strom verbraucht wird</t>
+  </si>
+  <si>
+    <t>informatiker</t>
+  </si>
+  <si>
+    <t>entwickler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entwickler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thermostat nicht gefunden. api gebrochen </t>
+  </si>
+  <si>
+    <t>alle</t>
+  </si>
+  <si>
+    <t>Wie frage 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of scope für so nen chatbot. Fokus sollte eher auf Datenschutz sein. keine neuen Features in der app vorhanden. privacy </t>
+  </si>
+  <si>
+    <t>example of possible questions would be nice to show. a voice option would be nice. maybe more style in the text bold etc</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>true and would use it.</t>
+  </si>
+  <si>
+    <t>controlling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,8 +225,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -510,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC7524D-5D90-4BFF-9A25-A0B83F25E75B}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,21 +566,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>26</v>
@@ -558,6 +590,62 @@
       </c>
       <c r="D3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>58</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -567,15 +655,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB2C15A-A61B-4C41-9070-8D5A88F296C0}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="19" max="19" width="11.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -630,8 +721,12 @@
       <c r="R1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T1">
+        <f>AVERAGE(A:A)</f>
+        <v>16.333333333333332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
@@ -686,8 +781,12 @@
       <c r="R2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T2">
+        <f>AVERAGE(D:D)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>12</v>
       </c>
@@ -740,6 +839,246 @@
         <v>2</v>
       </c>
       <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <f>AVERAGE(G:G)</f>
+        <v>36.166666666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>15</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>29</v>
+      </c>
+      <c r="N4" s="1">
+        <v>3</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>3</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f>AVERAGE(J:J)</f>
+        <v>25.833333333333332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>25</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>20</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <f>AVERAGE(M:M)</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>41</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>25</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <f>AVERAGE(P:P)</f>
+        <v>26.833333333333332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>38</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>92</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>27</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>99</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>41</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
         <v>1</v>
       </c>
     </row>
@@ -751,15 +1090,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789C94B5-0D57-4747-B312-C62FB78DFB79}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -778,11 +1117,12 @@
       <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1">
+        <f>AVERAGE(A:A)</f>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -801,11 +1141,12 @@
       <c r="F2">
         <v>3</v>
       </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <f>AVERAGE(B:B)</f>
+        <v>4.333333333333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -822,6 +1163,102 @@
         <v>4</v>
       </c>
       <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <f>AVERAGE(C:C)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f>AVERAGE(D:D)</f>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <f>AVERAGE(E:E)</f>
+        <v>3.8333333333333335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(F:F)</f>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
     </row>
@@ -832,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113701EC-2195-4FFB-AE90-7F1ED35515DB}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,30 +1293,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>